<commit_message>
PullRequest: 123 一些 bug fix
Merge branch 'fix/dev-4.2.0-bugs-xyh-0802 of git@gitlab.alipay-inc.com:oceanbase/oceanbase-developer-center.git into dev-4.2.0

https://code.alipay.com/oceanbase/oceanbase-developer-center/pull_requests/123


Signed-off-by: 晓康 <xxk268858@oceanbase.com>


* docs: 数据源-批量导入（文案订正）

* chore: 数据源模版更新

* fix(100879923): 配置sso信息没填必填信息报错有误

* fix(100878706): 工单，sql计划tab栏目下的字模块都无法通过状态进行筛选

* chore: 批量导入用户（模版更新）

* fix(100874688): 当点击生成备份回滚方案后没有生成回滚工单时，还是可以点击引用系统生成回滚方案

* fix(100870068): 影子表工单描述没加 可选

* fix(100800924): 查看详情中的时间运算英文单位改为中文

* fix(100789043): 数据归档，时间运算为空时显示‘-’，非null

* fix(100788990): 创建周期执行数据归档，查看详情中的执行方式显示定时执行
</commit_message>
<xml_diff>
--- a/public/template/en-us/user_template.xlsx
+++ b/public/template/en-us/user_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fzzf/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gaoda/Documents/batch import template/user/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50554CCF-10B7-2D41-828B-485D9409141F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4080E7EB-92C1-5F43-AE3A-FFA15EF8144F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3160" yWindow="2160" windowWidth="28240" windowHeight="17440" xr2:uid="{29034D28-73C4-B942-810F-3A50AB83AFBE}"/>
   </bookViews>
@@ -37,27 +37,27 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
-    <t>accountName</t>
+    <t>Username</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>name</t>
+    <t>Password</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>password</t>
+    <t>Role</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>enabled</t>
+    <t>Comment</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>description</t>
+    <t>Account</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>roleNames</t>
+    <t>Account Status</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -65,7 +65,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -78,6 +78,22 @@
       <sz val="9"/>
       <name val="等线"/>
       <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="DengXian"/>
+      <family val="4"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="4"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -104,11 +120,26 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -425,44 +456,60 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E55E1AB-64C0-D549-B607-DE32685C8B43}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" style="1"/>
-    <col min="5" max="5" width="40" customWidth="1"/>
+    <col min="1" max="3" width="30.83203125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="30.83203125" style="1" customWidth="1"/>
+    <col min="5" max="6" width="30.83203125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" t="s">
+      <c r="A1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D1048576" xr:uid="{1AE33F30-531F-614E-98F8-8E6E21FCF35B}">
-      <formula1>#REF!</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D1048576" xr:uid="{0600850D-4C9D-384F-A925-4836FC3DEEC6}">
+      <formula1>"true,false"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>